<commit_message>
wiedemann, starting notes from 1st chapter
</commit_message>
<xml_diff>
--- a/GEH.xlsx
+++ b/GEH.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vanis-Sumo\thesis\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815"/>
   </bookViews>
@@ -33,7 +28,7 @@
     <definedName name="GEH_8" localSheetId="0">List2!$AI$2:$AI$25</definedName>
     <definedName name="GEH_9" localSheetId="0">List2!$AJ$2:$AJ$25</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -281,17 +276,7 @@
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -436,43 +421,43 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_11" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_4" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_10" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_7" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_7" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_2" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_2" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_3" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_2" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_10" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_9" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_9" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_5" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -480,23 +465,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_4" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_6" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_2" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_11" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_5" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GEH_6" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -754,7 +739,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -762,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO26"/>
+  <dimension ref="A1:AS26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView tabSelected="1" topLeftCell="Z4" workbookViewId="0">
+      <selection activeCell="AR21" sqref="AR21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +762,7 @@
     <col min="33" max="33" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="1">
         <v>218</v>
@@ -877,7 +862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>4.0972222222222222E-2</v>
       </c>
@@ -1005,8 +990,15 @@
         <f t="shared" si="3"/>
         <v>1.5491933384829668</v>
       </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ2">
+        <v>126</v>
+      </c>
+      <c r="AR2">
+        <f>SQRT(2*(AQ2-B2)^2/(AQ2+B2))</f>
+        <v>0.44108109139123092</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>8.2638888888888887E-2</v>
       </c>
@@ -1134,8 +1126,15 @@
         <f t="shared" si="3"/>
         <v>0.59119756689857594</v>
       </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ3">
+        <v>100</v>
+      </c>
+      <c r="AR3">
+        <f t="shared" ref="AR3:AR25" si="11">SQRT(2*(AQ3-B3)^2/(AQ3+B3))</f>
+        <v>0.40406101782088427</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>0.12430555555555556</v>
       </c>
@@ -1263,8 +1262,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ4">
+        <v>88</v>
+      </c>
+      <c r="AR4">
+        <f t="shared" si="11"/>
+        <v>0.10629880069054677</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>0.16597222222222222</v>
       </c>
@@ -1392,8 +1398,15 @@
         <f t="shared" si="3"/>
         <v>0.14990633779917228</v>
       </c>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ5">
+        <v>45</v>
+      </c>
+      <c r="AR5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>0.2076388888888889</v>
       </c>
@@ -1521,8 +1534,15 @@
         <f t="shared" si="3"/>
         <v>0.96609178307929588</v>
       </c>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ6">
+        <v>49</v>
+      </c>
+      <c r="AR6">
+        <f t="shared" si="11"/>
+        <v>0.28284271247461901</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>0.24930555555555556</v>
       </c>
@@ -1650,8 +1670,15 @@
         <f t="shared" si="3"/>
         <v>0.18814417367671946</v>
       </c>
-    </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ7">
+        <v>114</v>
+      </c>
+      <c r="AR7">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>0.29097222222222224</v>
       </c>
@@ -1779,8 +1806,15 @@
         <f t="shared" si="3"/>
         <v>0.58501793930170454</v>
       </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ8">
+        <v>183</v>
+      </c>
+      <c r="AR8">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>0.33263888888888887</v>
       </c>
@@ -1908,8 +1942,15 @@
         <f t="shared" si="3"/>
         <v>0.27972711943222972</v>
       </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ9">
+        <v>322</v>
+      </c>
+      <c r="AR9">
+        <f t="shared" si="11"/>
+        <v>0.71725843678871892</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>0.3743055555555555</v>
       </c>
@@ -2037,8 +2078,15 @@
         <f t="shared" si="3"/>
         <v>1.4836636618975407</v>
       </c>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ10">
+        <v>528</v>
+      </c>
+      <c r="AR10">
+        <f t="shared" si="11"/>
+        <v>1.0327955589886444</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>0.41597222222222219</v>
       </c>
@@ -2166,8 +2214,15 @@
         <f t="shared" si="3"/>
         <v>2.0923986518947637</v>
       </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ11">
+        <v>841</v>
+      </c>
+      <c r="AR11">
+        <f t="shared" si="11"/>
+        <v>1.1945322919963342</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>0.45763888888888887</v>
       </c>
@@ -2295,8 +2350,15 @@
         <f t="shared" si="3"/>
         <v>2.1007737902016825</v>
       </c>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ12">
+        <v>1177</v>
+      </c>
+      <c r="AR12">
+        <f t="shared" si="11"/>
+        <v>0.3488902827777482</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>0.4993055555555555</v>
       </c>
@@ -2424,8 +2486,15 @@
         <f t="shared" si="3"/>
         <v>0.68823271265445896</v>
       </c>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ13">
+        <v>1314</v>
+      </c>
+      <c r="AR13">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>0.54097222222222219</v>
       </c>
@@ -2553,8 +2622,15 @@
         <f t="shared" si="3"/>
         <v>2.3586408826243161</v>
       </c>
-    </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ14">
+        <v>1422</v>
+      </c>
+      <c r="AR14">
+        <f t="shared" si="11"/>
+        <v>0.97486637893910277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>0.58263888888888882</v>
       </c>
@@ -2682,8 +2758,15 @@
         <f t="shared" si="3"/>
         <v>1.5158063393251509</v>
       </c>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ15">
+        <v>1625</v>
+      </c>
+      <c r="AR15">
+        <f t="shared" si="11"/>
+        <v>1.1331286698889371</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>0.62430555555555556</v>
       </c>
@@ -2811,8 +2894,15 @@
         <f t="shared" si="3"/>
         <v>2.8539128059862433</v>
       </c>
-    </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ16">
+        <v>1793</v>
+      </c>
+      <c r="AR16">
+        <f t="shared" si="11"/>
+        <v>1.7066978964529029</v>
+      </c>
+    </row>
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>0.66597222222222219</v>
       </c>
@@ -2940,8 +3030,15 @@
         <f t="shared" si="3"/>
         <v>1.3902509350931551</v>
       </c>
-    </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ17">
+        <v>1908</v>
+      </c>
+      <c r="AR17">
+        <f t="shared" si="11"/>
+        <v>4.1798799567284828</v>
+      </c>
+    </row>
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>0.70763888888888893</v>
       </c>
@@ -3058,19 +3155,26 @@
         <v>0.65341026280354819</v>
       </c>
       <c r="AM18">
-        <f t="shared" ref="AM18:AM25" si="11">SQRT(2*(AI18-C18)^2/(AI18+C18))</f>
+        <f t="shared" ref="AM18:AM25" si="12">SQRT(2*(AI18-C18)^2/(AI18+C18))</f>
         <v>0.59010226492247497</v>
       </c>
       <c r="AN18">
-        <f t="shared" ref="AN18:AN25" si="12">SQRT(2*(AJ18-D18)^2/(AJ18+D18))</f>
+        <f t="shared" ref="AN18:AN25" si="13">SQRT(2*(AJ18-D18)^2/(AJ18+D18))</f>
         <v>1.5403874832306848</v>
       </c>
       <c r="AO18">
-        <f t="shared" ref="AO18:AO25" si="13">SQRT(2*(AK18-E18)^2/(AK18+E18))</f>
+        <f t="shared" ref="AO18:AO25" si="14">SQRT(2*(AK18-E18)^2/(AK18+E18))</f>
         <v>1.3234314996770673</v>
       </c>
-    </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ18">
+        <v>1779</v>
+      </c>
+      <c r="AR18">
+        <f t="shared" si="11"/>
+        <v>7.7880693100185292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>0.74930555555555556</v>
       </c>
@@ -3187,19 +3291,26 @@
         <v>2.4649819661138932</v>
       </c>
       <c r="AM19">
+        <f t="shared" si="12"/>
+        <v>3.2858096575374263</v>
+      </c>
+      <c r="AN19">
+        <f t="shared" si="13"/>
+        <v>2.0747996779911149</v>
+      </c>
+      <c r="AO19">
+        <f t="shared" si="14"/>
+        <v>1.8798094870482889</v>
+      </c>
+      <c r="AQ19">
+        <v>1769</v>
+      </c>
+      <c r="AR19">
         <f t="shared" si="11"/>
-        <v>3.2858096575374263</v>
-      </c>
-      <c r="AN19">
-        <f t="shared" si="12"/>
-        <v>2.0747996779911149</v>
-      </c>
-      <c r="AO19">
-        <f t="shared" si="13"/>
-        <v>1.8798094870482889</v>
-      </c>
-    </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+        <v>6.3202424067203582</v>
+      </c>
+    </row>
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>0.7909722222222223</v>
       </c>
@@ -3316,19 +3427,26 @@
         <v>1.3752148941171205</v>
       </c>
       <c r="AM20">
+        <f t="shared" si="12"/>
+        <v>1.0976016168318701</v>
+      </c>
+      <c r="AN20">
+        <f t="shared" si="13"/>
+        <v>1.6618098001125854</v>
+      </c>
+      <c r="AO20">
+        <f t="shared" si="14"/>
+        <v>2.2556976843120515</v>
+      </c>
+      <c r="AQ20">
+        <v>1793</v>
+      </c>
+      <c r="AR20">
         <f t="shared" si="11"/>
-        <v>1.0976016168318701</v>
-      </c>
-      <c r="AN20">
-        <f t="shared" si="12"/>
-        <v>1.6618098001125854</v>
-      </c>
-      <c r="AO20">
-        <f t="shared" si="13"/>
-        <v>2.2556976843120515</v>
-      </c>
-    </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+        <v>5.3878405833469296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>0.83263888888888893</v>
       </c>
@@ -3445,19 +3563,26 @@
         <v>1.7945057741909052</v>
       </c>
       <c r="AM21">
+        <f t="shared" si="12"/>
+        <v>2.4962239702258229</v>
+      </c>
+      <c r="AN21">
+        <f t="shared" si="13"/>
+        <v>1.7245123251239711</v>
+      </c>
+      <c r="AO21">
+        <f t="shared" si="14"/>
+        <v>1.4900437824948636</v>
+      </c>
+      <c r="AQ21">
+        <v>1800</v>
+      </c>
+      <c r="AR21">
         <f t="shared" si="11"/>
-        <v>2.4962239702258229</v>
-      </c>
-      <c r="AN21">
-        <f t="shared" si="12"/>
-        <v>1.7245123251239711</v>
-      </c>
-      <c r="AO21">
-        <f t="shared" si="13"/>
-        <v>1.4900437824948636</v>
-      </c>
-    </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+        <v>17.650452162436562</v>
+      </c>
+    </row>
+    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>0.87430555555555556</v>
       </c>
@@ -3574,19 +3699,26 @@
         <v>0.38831088101434413</v>
       </c>
       <c r="AM22">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AN22">
+        <f t="shared" si="13"/>
+        <v>0.51399405296258838</v>
+      </c>
+      <c r="AO22">
+        <f t="shared" si="14"/>
+        <v>0.19215378456610457</v>
+      </c>
+      <c r="AQ22">
+        <v>1028</v>
+      </c>
+      <c r="AR22">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AN22">
-        <f t="shared" si="12"/>
-        <v>0.51399405296258838</v>
-      </c>
-      <c r="AO22">
-        <f t="shared" si="13"/>
-        <v>0.19215378456610457</v>
-      </c>
-    </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+        <v>2.512689092278678</v>
+      </c>
+    </row>
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>0.9159722222222223</v>
       </c>
@@ -3703,19 +3835,26 @@
         <v>0.20970306099501082</v>
       </c>
       <c r="AM23">
+        <f t="shared" si="12"/>
+        <v>0.92884072802564799</v>
+      </c>
+      <c r="AN23">
+        <f t="shared" si="13"/>
+        <v>0.29078454467808479</v>
+      </c>
+      <c r="AO23">
+        <f t="shared" si="14"/>
+        <v>0.49656353316142077</v>
+      </c>
+      <c r="AQ23">
+        <v>580</v>
+      </c>
+      <c r="AR23">
         <f t="shared" si="11"/>
-        <v>0.92884072802564799</v>
-      </c>
-      <c r="AN23">
-        <f t="shared" si="12"/>
-        <v>0.29078454467808479</v>
-      </c>
-      <c r="AO23">
-        <f t="shared" si="13"/>
-        <v>0.49656353316142077</v>
-      </c>
-    </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+        <v>0.58485839040209964</v>
+      </c>
+    </row>
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>0.95763888888888893</v>
       </c>
@@ -3832,19 +3971,26 @@
         <v>0</v>
       </c>
       <c r="AM24">
+        <f t="shared" si="12"/>
+        <v>5.3877245844036532E-2</v>
+      </c>
+      <c r="AN24">
+        <f t="shared" si="13"/>
+        <v>0.16070147520167405</v>
+      </c>
+      <c r="AO24">
+        <f t="shared" si="14"/>
+        <v>0.32209687625701139</v>
+      </c>
+      <c r="AQ24">
+        <v>350</v>
+      </c>
+      <c r="AR24">
         <f t="shared" si="11"/>
-        <v>5.3877245844036532E-2</v>
-      </c>
-      <c r="AN24">
-        <f t="shared" si="12"/>
-        <v>0.16070147520167405</v>
-      </c>
-      <c r="AO24">
-        <f t="shared" si="13"/>
-        <v>0.32209687625701139</v>
-      </c>
-    </row>
-    <row r="25" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.26822089039291003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>0.99930555555555556</v>
       </c>
@@ -3961,33 +4107,41 @@
         <v>0</v>
       </c>
       <c r="AM25">
+        <f t="shared" si="12"/>
+        <v>6.5163521245107464E-2</v>
+      </c>
+      <c r="AN25">
+        <f t="shared" si="13"/>
+        <v>0.39307306924825103</v>
+      </c>
+      <c r="AO25">
+        <f t="shared" si="14"/>
+        <v>0.59024325220555762</v>
+      </c>
+      <c r="AQ25" s="1">
+        <v>237</v>
+      </c>
+      <c r="AR25">
         <f t="shared" si="11"/>
-        <v>6.5163521245107464E-2</v>
-      </c>
-      <c r="AN25">
-        <f t="shared" si="12"/>
-        <v>0.39307306924825103</v>
-      </c>
-      <c r="AO25">
-        <f t="shared" si="13"/>
-        <v>0.59024325220555762</v>
-      </c>
-    </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+        <v>6.5025608876235513E-2</v>
+      </c>
+      <c r="AS25"/>
+    </row>
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="K26" s="8">
         <f>SUM(K2:K25)</f>
         <v>12.658694256461487</v>
       </c>
       <c r="L26" s="8">
-        <f t="shared" ref="L26:N26" si="14">SUM(L2:L25)</f>
+        <f t="shared" ref="L26:N26" si="15">SUM(L2:L25)</f>
         <v>19.514503141524173</v>
       </c>
       <c r="M26" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>29.426087445030632</v>
       </c>
       <c r="N26" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>27.342997938070337</v>
       </c>
       <c r="T26" s="8">
@@ -3995,15 +4149,15 @@
         <v>12.426673714591196</v>
       </c>
       <c r="U26" s="8">
-        <f t="shared" ref="U26" si="15">SUM(U2:U25)</f>
+        <f t="shared" ref="U26" si="16">SUM(U2:U25)</f>
         <v>19.669891420532764</v>
       </c>
       <c r="V26" s="8">
-        <f t="shared" ref="V26" si="16">SUM(V2:V25)</f>
+        <f t="shared" ref="V26" si="17">SUM(V2:V25)</f>
         <v>29.894972682022328</v>
       </c>
       <c r="W26" s="8">
-        <f t="shared" ref="W26" si="17">SUM(W2:W25)</f>
+        <f t="shared" ref="W26" si="18">SUM(W2:W25)</f>
         <v>27.993421599869393</v>
       </c>
       <c r="AC26" s="8">
@@ -4011,21 +4165,57 @@
         <v>12.039014807954635</v>
       </c>
       <c r="AD26" s="8">
-        <f t="shared" ref="AD26" si="18">SUM(AD2:AD25)</f>
+        <f t="shared" ref="AD26" si="19">SUM(AD2:AD25)</f>
         <v>20.010471483549853</v>
       </c>
       <c r="AE26" s="8">
-        <f t="shared" ref="AE26" si="19">SUM(AE2:AE25)</f>
+        <f t="shared" ref="AE26" si="20">SUM(AE2:AE25)</f>
         <v>29.141777404880102</v>
       </c>
       <c r="AF26" s="8">
-        <f t="shared" ref="AF26" si="20">SUM(AF2:AF25)</f>
+        <f t="shared" ref="AF26" si="21">SUM(AF2:AF25)</f>
         <v>27.473325232535274</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K26:K1048576 L26:N26">
-    <cfRule type="cellIs" dxfId="13" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="25" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" priority="27" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T2:W25">
+    <cfRule type="cellIs" dxfId="11" priority="22" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" priority="24" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC2:AF25">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
     <cfRule type="colorScale" priority="20">
@@ -4042,8 +4232,8 @@
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T2:W25">
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="greaterThan">
+  <conditionalFormatting sqref="T26:W26">
+    <cfRule type="cellIs" dxfId="9" priority="16" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
     <cfRule type="colorScale" priority="17">
@@ -4060,8 +4250,8 @@
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AF25">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThan">
+  <conditionalFormatting sqref="AC26:AF26">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
     <cfRule type="colorScale" priority="14">
@@ -4078,8 +4268,8 @@
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T26:W26">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
+  <conditionalFormatting sqref="K2:N25">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
     <cfRule type="colorScale" priority="11">
@@ -4096,8 +4286,8 @@
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC26:AF26">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
+  <conditionalFormatting sqref="AL2:AO25">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
     <cfRule type="colorScale" priority="8">
@@ -4114,7 +4304,7 @@
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:N25">
+  <conditionalFormatting sqref="AS2:AS25">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
@@ -4132,8 +4322,8 @@
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL2:AO25">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="AR2:AR25">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">

</xml_diff>